<commit_message>
2-26-2024 updated and added pdf sanitize flag
</commit_message>
<xml_diff>
--- a/bofa/bofa_research_search_results.xlsx
+++ b/bofa/bofa_research_search_results.xlsx
@@ -656,7 +656,7 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.245Z</t>
+          <t>2024-02-26T13:03:26.504Z</t>
         </is>
       </c>
       <c r="T2" t="inlineStr"/>
@@ -770,7 +770,7 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.246Z</t>
+          <t>2024-02-26T13:03:26.504Z</t>
         </is>
       </c>
       <c r="T3" t="inlineStr"/>
@@ -896,7 +896,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.246Z</t>
+          <t>2024-02-26T13:03:26.504Z</t>
         </is>
       </c>
       <c r="T4" t="inlineStr"/>
@@ -1022,7 +1022,7 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.246Z</t>
+          <t>2024-02-26T13:03:26.504Z</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.246Z</t>
+          <t>2024-02-26T13:03:26.504Z</t>
         </is>
       </c>
       <c r="T6" t="inlineStr"/>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.246Z</t>
+          <t>2024-02-26T13:03:26.504Z</t>
         </is>
       </c>
       <c r="T7" t="inlineStr"/>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.246Z</t>
+          <t>2024-02-26T13:03:26.504Z</t>
         </is>
       </c>
       <c r="T8" t="inlineStr"/>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.246Z</t>
+          <t>2024-02-26T13:03:26.504Z</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.246Z</t>
+          <t>2024-02-26T13:03:26.504Z</t>
         </is>
       </c>
       <c r="T10" t="inlineStr"/>
@@ -1770,7 +1770,7 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.246Z</t>
+          <t>2024-02-26T13:03:26.504Z</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
@@ -1908,7 +1908,7 @@
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.246Z</t>
+          <t>2024-02-26T13:03:26.504Z</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.246Z</t>
+          <t>2024-02-26T13:03:26.505Z</t>
         </is>
       </c>
       <c r="T13" t="inlineStr"/>
@@ -2160,7 +2160,7 @@
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.246Z</t>
+          <t>2024-02-26T13:03:26.505Z</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
@@ -2298,7 +2298,7 @@
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.246Z</t>
+          <t>2024-02-26T13:03:26.505Z</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.246Z</t>
+          <t>2024-02-26T13:03:26.505Z</t>
         </is>
       </c>
       <c r="T16" t="inlineStr"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.247Z</t>
+          <t>2024-02-26T13:03:26.505Z</t>
         </is>
       </c>
       <c r="T17" t="inlineStr"/>
@@ -2660,7 +2660,7 @@
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.247Z</t>
+          <t>2024-02-26T13:03:26.505Z</t>
         </is>
       </c>
       <c r="T18" t="inlineStr"/>
@@ -2786,7 +2786,7 @@
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.247Z</t>
+          <t>2024-02-26T13:03:26.505Z</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
@@ -2912,7 +2912,7 @@
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.247Z</t>
+          <t>2024-02-26T13:03:26.505Z</t>
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
@@ -3038,7 +3038,7 @@
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.247Z</t>
+          <t>2024-02-26T13:03:26.505Z</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
@@ -3168,7 +3168,7 @@
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>2024-02-25T20:28:33.247Z</t>
+          <t>2024-02-26T13:03:26.505Z</t>
         </is>
       </c>
       <c r="T22" t="inlineStr"/>

</xml_diff>